<commit_message>
Autor: Laura Descripcion: Se realizo la automatización de Avances de tarjeta de credito por los dos flujos fecha: 14/11/2019
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/Avances.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/Avances.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\Desktop\proyecto laura\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\avacestarjetacredito\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\git\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\avacestarjetacredito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668CEA70-ED25-48CA-949B-BFF3C1FF10A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1308DD-65A4-44E8-920E-DA656EC7EC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
-    <sheet name="Listas" sheetId="2" r:id="rId2"/>
+    <sheet name="DatosAvanceNoExitoso" sheetId="3" r:id="rId2"/>
+    <sheet name="Listas" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -134,25 +135,55 @@
     <t>Consultas</t>
   </si>
   <si>
+    <t>codigoSeguridad</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>American Express Blu</t>
+  </si>
+  <si>
+    <t>Visa Clásica</t>
+  </si>
+  <si>
+    <t>TUTAINABANCOLOMBIA10</t>
+  </si>
+  <si>
+    <t>numeroTarjetaDestino</t>
+  </si>
+  <si>
+    <t>406-110100-01</t>
+  </si>
+  <si>
+    <t>mensajeConfirmacion</t>
+  </si>
+  <si>
+    <t>¡Avance exitoso!</t>
+  </si>
+  <si>
+    <t>montoAvance</t>
+  </si>
+  <si>
+    <t>TUTAINABANCOLOMBIA11</t>
+  </si>
+  <si>
+    <t>406-110100-02</t>
+  </si>
+  <si>
+    <t>numeroTarjeta</t>
+  </si>
+  <si>
+    <t>mensajeAvanceNoExitoso</t>
+  </si>
+  <si>
+    <t>Cupo insuficiente</t>
+  </si>
+  <si>
+    <t>mensajeNoExitoso</t>
+  </si>
+  <si>
     <t>testing10</t>
-  </si>
-  <si>
-    <t>nuemeroTarjeta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Master Card Clásica </t>
-  </si>
-  <si>
-    <t>codigoSeguridad</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>American Express Blu</t>
-  </si>
-  <si>
-    <t>Visa Clásica</t>
   </si>
 </sst>
 </file>
@@ -223,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -246,12 +277,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -260,13 +304,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -561,9 +604,13 @@
     <col min="12" max="12" width="14.625" customWidth="1"/>
     <col min="13" max="13" width="18.5" customWidth="1"/>
     <col min="14" max="14" width="19.375" customWidth="1"/>
+    <col min="15" max="15" width="26.875" customWidth="1"/>
+    <col min="16" max="16" width="27.75" customWidth="1"/>
+    <col min="17" max="17" width="28.375" customWidth="1"/>
+    <col min="18" max="18" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,24 +648,36 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>37</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>48349402</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>13</v>
@@ -647,22 +706,34 @@
       <c r="M2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="7">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="N2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="O2" s="7">
+        <v>250000</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="9">
+        <v>48349402</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="11">
-        <v>48349402</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>13</v>
@@ -689,24 +760,36 @@
         <v>20</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="7">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="11">
+        <v>40</v>
+      </c>
+      <c r="N3" s="11">
+        <v>123</v>
+      </c>
+      <c r="O3" s="7">
+        <v>150000</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>48349402</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>37</v>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
@@ -733,24 +816,36 @@
         <v>20</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="7">
+        <v>39</v>
+      </c>
+      <c r="N4" s="11">
         <v>1234</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="11">
+      <c r="O4" s="7">
+        <v>50000</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>48349402</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>37</v>
+      <c r="D5" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>13</v>
@@ -777,23 +872,194 @@
         <v>20</v>
       </c>
       <c r="M5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="11">
+        <v>123</v>
+      </c>
+      <c r="O5" s="7">
+        <v>150000000</v>
+      </c>
+      <c r="P5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="7">
+      <c r="Q5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>48349402</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="11">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="C7" s="10"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="L9" s="10"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="D13" s="12"/>
+      <c r="O6" s="7">
+        <v>3000000</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>48349402</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="11">
+        <v>123</v>
+      </c>
+      <c r="O7" s="7">
+        <v>1500000</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9">
+        <v>48349402</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="11">
+        <v>123</v>
+      </c>
+      <c r="O8" s="7">
+        <v>1500000</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="D12" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -806,7 +1072,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:J5</xm:sqref>
+          <xm:sqref>G2:J8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -815,6 +1081,136 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A0F862-4422-4A87-8824-CCF7A658CD43}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="16" max="16" width="19.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9">
+        <v>48349402</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="O2" s="7">
+        <v>150000000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D4A1A0BB-2604-4723-8702-65053F6DAA30}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Se realiza modificación, flujo Enviar dinero Autor: Laura echeverry Fecha: 12/04/2019
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/Avances.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/Avances.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\git\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\avacestarjetacredito\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AA2F74-056E-4307-A7E7-2420FA47BD38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -182,13 +183,16 @@
   </si>
   <si>
     <t>*8078</t>
+  </si>
+  <si>
+    <t>406-139740-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -311,7 +315,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -583,32 +587,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" customWidth="1"/>
-    <col min="5" max="6" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.1640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="33.125" customWidth="1"/>
+    <col min="5" max="6" width="14.375" customWidth="1"/>
+    <col min="9" max="9" width="18.375" customWidth="1"/>
+    <col min="10" max="10" width="22.125" customWidth="1"/>
+    <col min="11" max="11" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
     <col min="13" max="13" width="18.5" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" customWidth="1"/>
-    <col min="16" max="16" width="27.6640625" customWidth="1"/>
-    <col min="17" max="17" width="28.33203125" customWidth="1"/>
+    <col min="14" max="14" width="19.375" customWidth="1"/>
+    <col min="15" max="15" width="26.875" customWidth="1"/>
+    <col min="16" max="16" width="27.625" customWidth="1"/>
+    <col min="17" max="17" width="28.375" customWidth="1"/>
     <col min="18" max="18" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +668,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -711,7 +715,7 @@
         <v>250000</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>43</v>
@@ -720,7 +724,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="6" t="s">
         <v>38</v>
       </c>
@@ -776,7 +780,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -832,7 +836,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -888,7 +892,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -944,7 +948,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18">
       <c r="D12" s="10"/>
     </row>
   </sheetData>
@@ -1066,7 +1070,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1079,19 +1083,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="16" max="16" width="19.1640625" customWidth="1"/>
+    <col min="16" max="16" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1145,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1196,7 +1200,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1209,22 +1213,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1252,7 +1256,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1266,7 +1270,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -1274,17 +1278,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Autor: Laura Maria Echevery Fecha: 5/12/2019 Descripción: Se Realizo automatización ATC Android
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/Avances.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/Avances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\git\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\avacestarjetacredito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AA2F74-056E-4307-A7E7-2420FA47BD38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7A95AF-31D9-49B0-B9D5-1A3EB55F14F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>numeroTarjetaDestino</t>
-  </si>
-  <si>
-    <t>406-110100-01</t>
   </si>
   <si>
     <t>mensajeConfirmacion</t>
@@ -591,7 +588,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -650,22 +647,22 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -679,7 +676,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>13</v>
@@ -709,19 +706,19 @@
         <v>50</v>
       </c>
       <c r="N2" s="11">
-        <v>1234</v>
+        <v>123</v>
       </c>
       <c r="O2" s="7">
         <v>250000</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -735,7 +732,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>13</v>
@@ -762,22 +759,22 @@
         <v>20</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N3" s="11">
-        <v>123</v>
+        <v>1234</v>
       </c>
       <c r="O3" s="7">
         <v>150000</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -791,7 +788,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
@@ -818,7 +815,7 @@
         <v>20</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N4" s="11">
         <v>1234</v>
@@ -827,13 +824,13 @@
         <v>50000</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -847,7 +844,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>13</v>
@@ -874,7 +871,7 @@
         <v>20</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N5" s="11">
         <v>123</v>
@@ -883,13 +880,13 @@
         <v>150000000</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -903,7 +900,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>13</v>
@@ -930,7 +927,7 @@
         <v>20</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N6" s="11">
         <v>123</v>
@@ -939,13 +936,13 @@
         <v>3000000</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -959,7 +956,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>13</v>
@@ -986,7 +983,7 @@
         <v>20</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N7" s="11">
         <v>123</v>
@@ -995,13 +992,13 @@
         <v>1500000</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1015,7 +1012,7 @@
         <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>13</v>
@@ -1042,7 +1039,7 @@
         <v>20</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N8" s="11">
         <v>123</v>
@@ -1051,13 +1048,13 @@
         <v>1500000</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1133,16 +1130,16 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1156,7 +1153,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>13</v>
@@ -1192,7 +1189,7 @@
         <v>150000000</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se estabiliza la transacciòn de avances solicitada
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/Avances.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/Avances.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\git\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\avacestarjetacredito\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/avacestarjetacredito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7A95AF-31D9-49B0-B9D5-1A3EB55F14F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="DatosAvanceNoExitoso" sheetId="3" r:id="rId2"/>
     <sheet name="Listas" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -176,20 +175,26 @@
     <t>testing10</t>
   </si>
   <si>
-    <t>*6889</t>
-  </si>
-  <si>
     <t>*8078</t>
   </si>
   <si>
-    <t>406-139740-01</t>
+    <t>avancestdc8</t>
+  </si>
+  <si>
+    <t>*6716</t>
+  </si>
+  <si>
+    <t>*2442</t>
+  </si>
+  <si>
+    <t>406-110080-05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,7 +317,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -584,32 +589,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="3" width="14.375" customWidth="1"/>
-    <col min="4" max="4" width="33.125" customWidth="1"/>
-    <col min="5" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.1640625" customWidth="1"/>
+    <col min="5" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
     <col min="13" max="13" width="18.5" customWidth="1"/>
-    <col min="14" max="14" width="19.375" customWidth="1"/>
-    <col min="15" max="15" width="26.875" customWidth="1"/>
-    <col min="16" max="16" width="27.625" customWidth="1"/>
-    <col min="17" max="17" width="28.375" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" customWidth="1"/>
+    <col min="17" max="17" width="28.33203125" customWidth="1"/>
     <col min="18" max="18" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,7 +670,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -676,7 +681,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>13</v>
@@ -703,16 +708,16 @@
         <v>20</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N2" s="11">
-        <v>123</v>
+        <v>314</v>
       </c>
       <c r="O2" s="7">
         <v>250000</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>42</v>
@@ -721,7 +726,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>38</v>
       </c>
@@ -732,7 +737,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>13</v>
@@ -759,16 +764,16 @@
         <v>20</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N3" s="11">
-        <v>1234</v>
+        <v>9639</v>
       </c>
       <c r="O3" s="7">
         <v>150000</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>42</v>
@@ -777,7 +782,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -788,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
@@ -815,16 +820,16 @@
         <v>20</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="N4" s="11">
-        <v>1234</v>
+        <v>314</v>
       </c>
       <c r="O4" s="7">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>42</v>
@@ -833,7 +838,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -844,7 +849,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>13</v>
@@ -871,16 +876,16 @@
         <v>20</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N5" s="11">
-        <v>123</v>
+        <v>9639</v>
       </c>
       <c r="O5" s="7">
-        <v>150000000</v>
+        <v>1300000</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q5" s="7" t="s">
         <v>42</v>
@@ -889,7 +894,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -900,7 +905,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>13</v>
@@ -927,16 +932,16 @@
         <v>20</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N6" s="11">
-        <v>123</v>
+        <v>9639</v>
       </c>
       <c r="O6" s="7">
-        <v>3000000</v>
+        <v>1187500</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>42</v>
@@ -945,120 +950,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9">
-        <v>48349402</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="11">
-        <v>123</v>
-      </c>
-      <c r="O7" s="7">
-        <v>1500000</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="9">
-        <v>6</v>
-      </c>
-      <c r="B8" s="9">
-        <v>48349402</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="11">
-        <v>123</v>
-      </c>
-      <c r="O8" s="7">
-        <v>1500000</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="D12" s="10"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D10" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1067,11 +960,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:J8</xm:sqref>
+          <xm:sqref>G2:J6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1080,19 +973,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="16" max="16" width="19.125" customWidth="1"/>
+    <col min="16" max="16" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1035,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1197,7 +1090,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1210,22 +1103,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1239,7 +1132,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1253,7 +1146,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1267,7 +1160,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -1275,17 +1168,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>36</v>
       </c>

</xml_diff>